<commit_message>
TP2B casi resuelto, faltan casos de prueba
</commit_message>
<xml_diff>
--- a/TP2B/Documentacion/PlanillaDeMetricas.xlsx
+++ b/TP2B/Documentacion/PlanillaDeMetricas.xlsx
@@ -1,15 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gmartin\Desktop\progra\pa-group\TP2B\Documentacion\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="240" yWindow="75" windowWidth="20730" windowHeight="10110"/>
   </bookViews>
   <sheets>
     <sheet name="Métricas" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -19,7 +24,7 @@
     <author>Gonzalo Martin</author>
   </authors>
   <commentList>
-    <comment ref="K15" authorId="0">
+    <comment ref="K15" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -43,7 +48,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="K16" authorId="0">
+    <comment ref="K16" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -848,53 +853,95 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -904,75 +951,13 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="6" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="6" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Porcentaje" xfId="1" builtinId="5"/>
   </cellStyles>
-  <dxfs count="4">
-    <dxf>
-      <font>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC00000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color auto="1"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <font>
         <color theme="0"/>
@@ -1009,6 +994,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1016,7 +1004,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
-  <c:lang val="es-AR"/>
+  <c:lang val="es-ES"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -1126,13 +1114,13 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>6.5972222222222265E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.2500000000000003E-3</c:v>
+                  <c:v>1.5972222222222221E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>0.12847222222222215</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1260,7 +1248,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1295,7 +1283,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1506,8 +1494,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
-      <selection activeCell="M20" sqref="M20"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" zoomScaleSheetLayoutView="115" workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1525,29 +1513,29 @@
       <c r="B1" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="C1" s="54" t="s">
+      <c r="C1" s="80" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
-      <c r="K1" s="54"/>
-      <c r="L1" s="54"/>
-      <c r="M1" s="54"/>
-      <c r="N1" s="54"/>
+      <c r="D1" s="80"/>
+      <c r="E1" s="80"/>
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="80"/>
+      <c r="I1" s="80"/>
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="80"/>
+      <c r="M1" s="80"/>
+      <c r="N1" s="80"/>
     </row>
     <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="13"/>
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="61" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="56"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57"/>
+      <c r="C2" s="62"/>
+      <c r="D2" s="62"/>
+      <c r="E2" s="63"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -1573,15 +1561,15 @@
       <c r="E3" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F3" s="65"/>
-      <c r="G3" s="65"/>
-      <c r="H3" s="65"/>
-      <c r="I3" s="65"/>
-      <c r="J3" s="65"/>
-      <c r="K3" s="65"/>
-      <c r="L3" s="65"/>
-      <c r="M3" s="65"/>
-      <c r="N3" s="65"/>
+      <c r="F3" s="82"/>
+      <c r="G3" s="82"/>
+      <c r="H3" s="82"/>
+      <c r="I3" s="82"/>
+      <c r="J3" s="82"/>
+      <c r="K3" s="82"/>
+      <c r="L3" s="82"/>
+      <c r="M3" s="82"/>
+      <c r="N3" s="82"/>
       <c r="O3" s="14"/>
       <c r="P3" s="9"/>
     </row>
@@ -1600,15 +1588,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C4),ISBLANK(D4)),"Completar",IF(D4&gt;=C4,D4-C4,"Error")),"Error")</f>
         <v>3.4722222222222099E-3</v>
       </c>
-      <c r="F4" s="66"/>
-      <c r="G4" s="66"/>
-      <c r="H4" s="66"/>
-      <c r="I4" s="66"/>
-      <c r="J4" s="66"/>
-      <c r="K4" s="66"/>
-      <c r="L4" s="66"/>
-      <c r="M4" s="66"/>
-      <c r="N4" s="66"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
       <c r="O4" s="15"/>
       <c r="P4" s="11"/>
     </row>
@@ -1632,12 +1620,12 @@
     </row>
     <row r="6" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="13"/>
-      <c r="B6" s="55" t="s">
+      <c r="B6" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="C6" s="56"/>
-      <c r="D6" s="56"/>
-      <c r="E6" s="57"/>
+      <c r="C6" s="62"/>
+      <c r="D6" s="62"/>
+      <c r="E6" s="63"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
       <c r="H6" s="12"/>
@@ -1663,15 +1651,15 @@
       <c r="E7" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="F7" s="65"/>
-      <c r="G7" s="65"/>
-      <c r="H7" s="65"/>
-      <c r="I7" s="65"/>
-      <c r="J7" s="65"/>
-      <c r="K7" s="65"/>
-      <c r="L7" s="65"/>
-      <c r="M7" s="65"/>
-      <c r="N7" s="65"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="82"/>
+      <c r="N7" s="82"/>
       <c r="O7" s="14"/>
       <c r="P7" s="9"/>
     </row>
@@ -1686,15 +1674,15 @@
         <f>IFERROR(IF(OR(ISBLANK(C8),ISBLANK(D8)),"Completar",IF(D8&gt;=C8,D8-C8,"Error")),"Error")</f>
         <v>Completar</v>
       </c>
-      <c r="F8" s="66"/>
-      <c r="G8" s="66"/>
-      <c r="H8" s="66"/>
-      <c r="I8" s="66"/>
-      <c r="J8" s="66"/>
-      <c r="K8" s="66"/>
-      <c r="L8" s="66"/>
-      <c r="M8" s="66"/>
-      <c r="N8" s="66"/>
+      <c r="F8" s="64"/>
+      <c r="G8" s="64"/>
+      <c r="H8" s="64"/>
+      <c r="I8" s="64"/>
+      <c r="J8" s="64"/>
+      <c r="K8" s="64"/>
+      <c r="L8" s="64"/>
+      <c r="M8" s="64"/>
+      <c r="N8" s="64"/>
       <c r="O8" s="15"/>
       <c r="P8" s="11"/>
     </row>
@@ -1718,50 +1706,50 @@
     </row>
     <row r="10" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="13"/>
-      <c r="B10" s="55" t="s">
+      <c r="B10" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="56"/>
-      <c r="D10" s="56"/>
-      <c r="E10" s="56"/>
-      <c r="F10" s="56"/>
-      <c r="G10" s="56"/>
-      <c r="H10" s="56"/>
-      <c r="I10" s="56"/>
-      <c r="J10" s="56"/>
-      <c r="K10" s="56"/>
-      <c r="L10" s="56"/>
-      <c r="M10" s="56"/>
-      <c r="N10" s="57"/>
+      <c r="C10" s="62"/>
+      <c r="D10" s="62"/>
+      <c r="E10" s="62"/>
+      <c r="F10" s="62"/>
+      <c r="G10" s="62"/>
+      <c r="H10" s="62"/>
+      <c r="I10" s="62"/>
+      <c r="J10" s="62"/>
+      <c r="K10" s="62"/>
+      <c r="L10" s="62"/>
+      <c r="M10" s="62"/>
+      <c r="N10" s="63"/>
       <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:16" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14"/>
-      <c r="B11" s="78" t="s">
+      <c r="B11" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="72" t="s">
+      <c r="C11" s="74" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="72"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="61" t="s">
+      <c r="D11" s="74"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="62"/>
-      <c r="H11" s="63" t="s">
+      <c r="G11" s="77"/>
+      <c r="H11" s="73" t="s">
         <v>14</v>
       </c>
-      <c r="I11" s="72"/>
-      <c r="J11" s="73"/>
-      <c r="K11" s="61" t="s">
+      <c r="I11" s="74"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76" t="s">
         <v>16</v>
       </c>
-      <c r="L11" s="62"/>
-      <c r="M11" s="63" t="s">
+      <c r="L11" s="77"/>
+      <c r="M11" s="73" t="s">
         <v>18</v>
       </c>
-      <c r="N11" s="64" t="s">
+      <c r="N11" s="81" t="s">
         <v>2</v>
       </c>
       <c r="O11" s="14"/>
@@ -1769,10 +1757,10 @@
     </row>
     <row r="12" spans="1:16" s="5" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="14"/>
-      <c r="B12" s="78"/>
-      <c r="C12" s="72"/>
-      <c r="D12" s="72"/>
-      <c r="E12" s="73"/>
+      <c r="B12" s="65"/>
+      <c r="C12" s="74"/>
+      <c r="D12" s="74"/>
+      <c r="E12" s="75"/>
       <c r="F12" s="18" t="s">
         <v>13</v>
       </c>
@@ -1794,8 +1782,8 @@
       <c r="L12" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="M12" s="63"/>
-      <c r="N12" s="64"/>
+      <c r="M12" s="73"/>
+      <c r="N12" s="81"/>
       <c r="O12" s="14"/>
       <c r="P12" s="9"/>
     </row>
@@ -1805,11 +1793,11 @@
         <f>ROW($B13)-12</f>
         <v>1</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="78" t="s">
         <v>32</v>
       </c>
-      <c r="D13" s="67"/>
-      <c r="E13" s="68"/>
+      <c r="D13" s="78"/>
+      <c r="E13" s="79"/>
       <c r="F13" s="47">
         <v>15</v>
       </c>
@@ -1848,11 +1836,11 @@
         <f t="shared" ref="B14:B15" si="0">ROW($B14)-12</f>
         <v>2</v>
       </c>
-      <c r="C14" s="67" t="s">
+      <c r="C14" s="78" t="s">
         <v>33</v>
       </c>
-      <c r="D14" s="67"/>
-      <c r="E14" s="68"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="79"/>
       <c r="F14" s="47">
         <v>15</v>
       </c>
@@ -1891,11 +1879,11 @@
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="C15" s="67" t="s">
+      <c r="C15" s="78" t="s">
         <v>34</v>
       </c>
-      <c r="D15" s="67"/>
-      <c r="E15" s="68"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="79"/>
       <c r="F15" s="47">
         <v>20</v>
       </c>
@@ -1934,11 +1922,11 @@
         <f>ROW($B16)-12</f>
         <v>4</v>
       </c>
-      <c r="C16" s="67" t="s">
+      <c r="C16" s="78" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="67"/>
-      <c r="E16" s="68"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="79"/>
       <c r="F16" s="47">
         <v>20</v>
       </c>
@@ -1977,27 +1965,39 @@
         <f>ROW($B17)-12</f>
         <v>5</v>
       </c>
-      <c r="C17" s="67" t="s">
+      <c r="C17" s="78" t="s">
         <v>36</v>
       </c>
-      <c r="D17" s="67"/>
-      <c r="E17" s="68"/>
+      <c r="D17" s="78"/>
+      <c r="E17" s="79"/>
       <c r="F17" s="47">
         <v>60</v>
       </c>
-      <c r="G17" s="48"/>
-      <c r="H17" s="49"/>
-      <c r="I17" s="50"/>
-      <c r="J17" s="20" t="str">
+      <c r="G17" s="48">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="H17" s="49">
+        <v>0.3611111111111111</v>
+      </c>
+      <c r="I17" s="50">
+        <v>0.40277777777777773</v>
+      </c>
+      <c r="J17" s="20">
         <f t="shared" ref="J17:J18" si="3">IFERROR(IF(OR(ISBLANK(H17),ISBLANK(I17)),"Completar",IF(I17&gt;=H17,I17-H17,"Error")),"Error")</f>
-        <v>Completar</v>
-      </c>
-      <c r="K17" s="51"/>
-      <c r="L17" s="52"/>
-      <c r="M17" s="53"/>
-      <c r="N17" s="25" t="str">
+        <v>4.166666666666663E-2</v>
+      </c>
+      <c r="K17" s="51">
+        <v>1</v>
+      </c>
+      <c r="L17" s="52">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="M17" s="53">
+        <v>50</v>
+      </c>
+      <c r="N17" s="25">
         <f t="shared" ref="N17:N18" si="4">IFERROR(IF(OR(J17="Completar",ISBLANK(L17)),"Completar",J17+L17),"Error")</f>
-        <v>Completar</v>
+        <v>4.8611111111111077E-2</v>
       </c>
       <c r="O17" s="14"/>
       <c r="P17" s="17"/>
@@ -2008,27 +2008,39 @@
         <f>ROW($B18)-12</f>
         <v>6</v>
       </c>
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="68"/>
+      <c r="D18" s="78"/>
+      <c r="E18" s="79"/>
       <c r="F18" s="47">
         <v>60</v>
       </c>
-      <c r="G18" s="48"/>
-      <c r="H18" s="49"/>
-      <c r="I18" s="50"/>
-      <c r="J18" s="20" t="str">
+      <c r="G18" s="48">
+        <v>2.4305555555555556E-2</v>
+      </c>
+      <c r="H18" s="49">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="I18" s="50">
+        <v>0.46527777777777773</v>
+      </c>
+      <c r="J18" s="20">
         <f t="shared" si="3"/>
-        <v>Completar</v>
-      </c>
-      <c r="K18" s="51"/>
-      <c r="L18" s="52"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="25" t="str">
+        <v>4.8611111111111049E-2</v>
+      </c>
+      <c r="K18" s="51">
+        <v>1</v>
+      </c>
+      <c r="L18" s="52">
+        <v>2.7777777777777779E-3</v>
+      </c>
+      <c r="M18" s="53">
+        <v>50</v>
+      </c>
+      <c r="N18" s="25">
         <f t="shared" si="4"/>
-        <v>Completar</v>
+        <v>5.1388888888888824E-2</v>
       </c>
       <c r="O18" s="16"/>
     </row>
@@ -2038,11 +2050,11 @@
         <f>ROW($B19)-12</f>
         <v>7</v>
       </c>
-      <c r="C19" s="67" t="s">
+      <c r="C19" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="D19" s="67"/>
-      <c r="E19" s="68"/>
+      <c r="D19" s="78"/>
+      <c r="E19" s="79"/>
       <c r="F19" s="47">
         <v>30</v>
       </c>
@@ -2076,41 +2088,41 @@
     </row>
     <row r="20" spans="1:16" s="2" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="13"/>
-      <c r="B20" s="69" t="s">
+      <c r="B20" s="83" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="70"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="71"/>
+      <c r="C20" s="84"/>
+      <c r="D20" s="84"/>
+      <c r="E20" s="85"/>
       <c r="F20" s="26">
         <f>SUM(F13:F19)</f>
         <v>220</v>
       </c>
       <c r="G20" s="27">
         <f>SUM(G13:G19)</f>
-        <v>3.888888888888889E-2</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="H20" s="28"/>
       <c r="I20" s="29"/>
-      <c r="J20" s="30" t="str">
+      <c r="J20" s="30">
         <f>IF(OR(COUNTIF(J13:J19,"Error")&gt;0,COUNTIF(J13:J19,"Completar")&gt;0),"Error",SUM(J13:J19))</f>
-        <v>Error</v>
+        <v>0.12847222222222215</v>
       </c>
       <c r="K20" s="31">
         <f>SUM(K13:K19)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L20" s="27">
         <f>SUM(L13:L19)</f>
-        <v>6.2500000000000003E-3</v>
+        <v>1.5972222222222221E-2</v>
       </c>
       <c r="M20" s="32">
         <f>SUM(M13:M19)</f>
-        <v>88</v>
-      </c>
-      <c r="N20" s="33" t="str">
+        <v>188</v>
+      </c>
+      <c r="N20" s="33">
         <f>IF(OR(COUNTIF(N13:N19,"Error")&gt;0,COUNTIF(N13:N19,"Completar")&gt;0),"Error",SUM(N13:N19))</f>
-        <v>Error</v>
+        <v>0.14444444444444438</v>
       </c>
       <c r="O20" s="13"/>
     </row>
@@ -2134,12 +2146,12 @@
     </row>
     <row r="22" spans="1:16" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15"/>
-      <c r="B22" s="55" t="s">
+      <c r="B22" s="61" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
-      <c r="E22" s="57"/>
+      <c r="C22" s="62"/>
+      <c r="D22" s="62"/>
+      <c r="E22" s="63"/>
       <c r="F22" s="12"/>
       <c r="G22" s="12"/>
       <c r="H22" s="12"/>
@@ -2178,12 +2190,18 @@
       <c r="O23" s="16"/>
     </row>
     <row r="24" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B24" s="45"/>
-      <c r="C24" s="46"/>
-      <c r="D24" s="46"/>
-      <c r="E24" s="33" t="str">
+      <c r="B24" s="45">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="C24" s="46">
+        <v>0.44791666666666669</v>
+      </c>
+      <c r="D24" s="46">
+        <v>0.51388888888888895</v>
+      </c>
+      <c r="E24" s="33">
         <f>IFERROR(IF(OR(ISBLANK(C24),ISBLANK(D24)),"Completar",IF(D24&gt;=C24,D24-C24,"Error")),"Error")</f>
-        <v>Completar</v>
+        <v>6.5972222222222265E-2</v>
       </c>
       <c r="F24" s="15"/>
       <c r="G24" s="15"/>
@@ -2211,33 +2229,33 @@
       <c r="N25" s="16"/>
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B26" s="55" t="s">
+      <c r="B26" s="61" t="s">
         <v>21</v>
       </c>
-      <c r="C26" s="56"/>
-      <c r="D26" s="56"/>
-      <c r="E26" s="56"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="56"/>
-      <c r="H26" s="56"/>
-      <c r="I26" s="56"/>
-      <c r="J26" s="56"/>
-      <c r="K26" s="56"/>
-      <c r="L26" s="56"/>
-      <c r="M26" s="56"/>
-      <c r="N26" s="57"/>
+      <c r="C26" s="62"/>
+      <c r="D26" s="62"/>
+      <c r="E26" s="62"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
+      <c r="H26" s="62"/>
+      <c r="I26" s="62"/>
+      <c r="J26" s="62"/>
+      <c r="K26" s="62"/>
+      <c r="L26" s="62"/>
+      <c r="M26" s="62"/>
+      <c r="N26" s="63"/>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B27" s="58" t="s">
+      <c r="B27" s="56" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="59"/>
-      <c r="D27" s="60"/>
-      <c r="E27" s="82">
+      <c r="C27" s="57"/>
+      <c r="D27" s="58"/>
+      <c r="E27" s="69">
         <f>M20</f>
-        <v>88</v>
-      </c>
-      <c r="F27" s="83"/>
+        <v>188</v>
+      </c>
+      <c r="F27" s="70"/>
       <c r="G27" s="34"/>
       <c r="H27" s="35"/>
       <c r="I27" s="35"/>
@@ -2248,16 +2266,16 @@
       <c r="N27" s="38"/>
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B28" s="58" t="s">
+      <c r="B28" s="56" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="59"/>
-      <c r="D28" s="60"/>
-      <c r="E28" s="84" t="str">
+      <c r="C28" s="57"/>
+      <c r="D28" s="58"/>
+      <c r="E28" s="71">
         <f>IF(M20=0,0,IFERROR(M20/(N20*24),"Error"))</f>
-        <v>Error</v>
-      </c>
-      <c r="F28" s="85"/>
+        <v>54.230769230769255</v>
+      </c>
+      <c r="F28" s="72"/>
       <c r="G28" s="36"/>
       <c r="H28" s="37"/>
       <c r="I28" s="37"/>
@@ -2268,16 +2286,16 @@
       <c r="N28" s="39"/>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B29" s="58" t="s">
+      <c r="B29" s="56" t="s">
         <v>22</v>
       </c>
-      <c r="C29" s="59"/>
-      <c r="D29" s="60"/>
-      <c r="E29" s="82">
+      <c r="C29" s="57"/>
+      <c r="D29" s="58"/>
+      <c r="E29" s="69">
         <f>IF(K20=0,0,IFERROR(ROUNDUP(K20/(M20/100),0),"Error"))</f>
         <v>3</v>
       </c>
-      <c r="F29" s="83"/>
+      <c r="F29" s="70"/>
       <c r="G29" s="36"/>
       <c r="H29" s="37"/>
       <c r="I29" s="37"/>
@@ -2288,16 +2306,16 @@
       <c r="N29" s="39"/>
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B30" s="58" t="s">
+      <c r="B30" s="56" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="59"/>
-      <c r="D30" s="60"/>
-      <c r="E30" s="74">
+      <c r="C30" s="57"/>
+      <c r="D30" s="58"/>
+      <c r="E30" s="54">
         <f>IF(K20=0,0,IFERROR(K20/M20,"Error"))</f>
-        <v>2.2727272727272728E-2</v>
-      </c>
-      <c r="F30" s="75"/>
+        <v>2.1276595744680851E-2</v>
+      </c>
+      <c r="F30" s="55"/>
       <c r="G30" s="36"/>
       <c r="H30" s="37"/>
       <c r="I30" s="37"/>
@@ -2308,18 +2326,18 @@
       <c r="N30" s="39"/>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B31" s="58" t="s">
+      <c r="B31" s="56" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="59"/>
-      <c r="D31" s="60"/>
+      <c r="C31" s="57"/>
+      <c r="D31" s="58"/>
       <c r="E31" s="43">
         <f>E4</f>
         <v>3.4722222222222099E-3</v>
       </c>
-      <c r="F31" s="44" t="str">
+      <c r="F31" s="44">
         <f t="shared" ref="F31:F35" si="5">IF(E31="Completar",E31,IFERROR(E31/$E$36,"Error"))</f>
-        <v>Error</v>
+        <v>1.623376623376618E-2</v>
       </c>
       <c r="G31" s="36"/>
       <c r="H31" s="37"/>
@@ -2331,11 +2349,11 @@
       <c r="N31" s="39"/>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="B32" s="58" t="s">
+      <c r="B32" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="C32" s="59"/>
-      <c r="D32" s="60"/>
+      <c r="C32" s="57"/>
+      <c r="D32" s="58"/>
       <c r="E32" s="43" t="str">
         <f>E8</f>
         <v>Completar</v>
@@ -2354,18 +2372,18 @@
       <c r="N32" s="39"/>
     </row>
     <row r="33" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B33" s="58" t="s">
+      <c r="B33" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="C33" s="59"/>
-      <c r="D33" s="60"/>
-      <c r="E33" s="43" t="str">
+      <c r="C33" s="57"/>
+      <c r="D33" s="58"/>
+      <c r="E33" s="43">
         <f>E24</f>
-        <v>Completar</v>
-      </c>
-      <c r="F33" s="44" t="str">
+        <v>6.5972222222222265E-2</v>
+      </c>
+      <c r="F33" s="44">
         <f>IF(E33="Completar",E33,IFERROR(E33/$E$36,"Error"))</f>
-        <v>Completar</v>
+        <v>0.30844155844155868</v>
       </c>
       <c r="G33" s="36"/>
       <c r="H33" s="37"/>
@@ -2377,18 +2395,18 @@
       <c r="N33" s="39"/>
     </row>
     <row r="34" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B34" s="58" t="s">
+      <c r="B34" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="60"/>
+      <c r="C34" s="57"/>
+      <c r="D34" s="58"/>
       <c r="E34" s="43">
         <f>L20</f>
-        <v>6.2500000000000003E-3</v>
-      </c>
-      <c r="F34" s="44" t="str">
+        <v>1.5972222222222221E-2</v>
+      </c>
+      <c r="F34" s="44">
         <f t="shared" si="5"/>
-        <v>Error</v>
+        <v>7.4675324675324686E-2</v>
       </c>
       <c r="G34" s="36"/>
       <c r="H34" s="37"/>
@@ -2401,18 +2419,18 @@
     </row>
     <row r="35" spans="1:15" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="16"/>
-      <c r="B35" s="58" t="s">
+      <c r="B35" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="C35" s="59"/>
-      <c r="D35" s="60"/>
-      <c r="E35" s="43" t="str">
+      <c r="C35" s="57"/>
+      <c r="D35" s="58"/>
+      <c r="E35" s="43">
         <f>J20</f>
-        <v>Error</v>
-      </c>
-      <c r="F35" s="44" t="str">
+        <v>0.12847222222222215</v>
+      </c>
+      <c r="F35" s="44">
         <f t="shared" si="5"/>
-        <v>Error</v>
+        <v>0.60064935064935043</v>
       </c>
       <c r="G35" s="36"/>
       <c r="H35" s="37"/>
@@ -2425,16 +2443,16 @@
       <c r="O35" s="16"/>
     </row>
     <row r="36" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="79" t="s">
+      <c r="B36" s="66" t="s">
         <v>6</v>
       </c>
-      <c r="C36" s="80"/>
-      <c r="D36" s="81"/>
-      <c r="E36" s="76" t="str">
+      <c r="C36" s="67"/>
+      <c r="D36" s="68"/>
+      <c r="E36" s="59">
         <f>IF(COUNTIF(E31:E35,"Error")=0,SUM(E31:E35),"Error")</f>
-        <v>Error</v>
-      </c>
-      <c r="F36" s="77"/>
+        <v>0.21388888888888885</v>
+      </c>
+      <c r="F36" s="60"/>
       <c r="G36" s="40"/>
       <c r="H36" s="41"/>
       <c r="I36" s="41"/>
@@ -2462,6 +2480,30 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="40">
+    <mergeCell ref="C1:N1"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B22:E22"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="M11:M12"/>
+    <mergeCell ref="N11:N12"/>
+    <mergeCell ref="F7:N7"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="B10:N10"/>
+    <mergeCell ref="C14:E14"/>
+    <mergeCell ref="C15:E15"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="B20:E20"/>
+    <mergeCell ref="F3:N3"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="C11:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="B28:D28"/>
+    <mergeCell ref="B29:D29"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="C16:E16"/>
+    <mergeCell ref="C18:E18"/>
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="E36:F36"/>
@@ -2478,36 +2520,12 @@
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="H11:J11"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="C11:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="B28:D28"/>
-    <mergeCell ref="B29:D29"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="C16:E16"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C1:N1"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B22:E22"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="M11:M12"/>
-    <mergeCell ref="N11:N12"/>
-    <mergeCell ref="F7:N7"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="B10:N10"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="C15:E15"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="B20:E20"/>
-    <mergeCell ref="F3:N3"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:XFD1048576">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
       <formula>"Completar"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="11" operator="equal">
       <formula>"Error"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>